<commit_message>
Add Batteries in addition to Ultracaps
</commit_message>
<xml_diff>
--- a/inputData/eco_cost_inputs_FG.xlsx
+++ b/inputData/eco_cost_inputs_FG.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\GitHubRepo\EcoModel\inputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\GitHubRepo\AWE-Eco\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F3B95E-BD25-4882-A4FB-698F1C25351E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622FB3A5-EB73-47EB-A39D-B9B6310050C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kite" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>[-2.4   8.3  -11.2   5.2]'</t>
   </si>
@@ -158,6 +158,15 @@
   </si>
   <si>
     <t>sigma_max</t>
+  </si>
+  <si>
+    <t>elecSto_type</t>
+  </si>
+  <si>
+    <t>batt.p</t>
+  </si>
+  <si>
+    <t>batt.N</t>
   </si>
 </sst>
 </file>
@@ -578,7 +587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF4AD09E-FDEF-4026-AC1D-93146C2A9B86}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -670,10 +679,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5144ACA-6792-40EA-A07E-EF86968317B7}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,50 +759,72 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="1">
-        <v>60000</v>
+        <v>34</v>
+      </c>
+      <c r="B9">
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>25</v>
       </c>
-      <c r="B10">
+      <c r="B14">
         <f>1000000</f>
         <v>1000000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13">
-        <v>100</v>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="1">
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16">
+        <f>10000</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Batt cost to 200 Euro/kWh
</commit_message>
<xml_diff>
--- a/inputData/eco_cost_inputs_FG.xlsx
+++ b/inputData/eco_cost_inputs_FG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\GitHubRepo\AWE-Eco\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622FB3A5-EB73-47EB-A39D-B9B6310050C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96514C06-B3F0-41D2-AC5F-0A6A1440305C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -682,7 +682,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,7 +811,7 @@
         <v>40</v>
       </c>
       <c r="B15" s="1">
-        <v>180</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update subsidy. IRR in percentage.
</commit_message>
<xml_diff>
--- a/inputData/eco_cost_inputs_FG.xlsx
+++ b/inputData/eco_cost_inputs_FG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\GitHubRepo\AWE-Eco\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33AE7A8-5C62-4885-A895-84028CCAF06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710B32DC-ADC8-4DBC-8291-046501D79B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kite" sheetId="3" r:id="rId1"/>
@@ -909,7 +909,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,7 +938,7 @@
         <v>29</v>
       </c>
       <c r="B3">
-        <v>200</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct Avonics cost per kW for FG
</commit_message>
<xml_diff>
--- a/inputData/eco_cost_inputs_FG.xlsx
+++ b/inputData/eco_cost_inputs_FG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\GitHubRepo\AWE-Eco\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710B32DC-ADC8-4DBC-8291-046501D79B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACBE3EB-810C-4A68-BE44-8C71035ECDED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kite" sheetId="3" r:id="rId1"/>
@@ -502,7 +502,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +572,7 @@
         <v>33</v>
       </c>
       <c r="B8" s="1">
-        <v>15000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -681,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5144ACA-6792-40EA-A07E-EF86968317B7}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +696,7 @@
         <v>10</v>
       </c>
       <c r="B1">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -908,7 +908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{149E8716-C12E-4C74-BB23-8FB9587F4C00}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>